<commit_message>
Aero sims and SN3 cell sims
</commit_message>
<xml_diff>
--- a/custom sim/full_acc_data_2.xlsx
+++ b/custom sim/full_acc_data_2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ddc151335309a76/Documents/GitHub/FEBSim/custom sim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EJDRO\OneDrive\Documents\GitHub\FEBSim\custom sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_28B5A2FDF613C8F64176303EF375C94C74524DD8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2D3E2AF2-8282-432D-BE51-0BD4D8F32004}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C818E794-F007-4C17-94E8-D7B0B2A65CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="45">
   <si>
     <t>Pack Config</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>rerun next month or 2</t>
+  </si>
+  <si>
+    <t>Average AutoX Times (s)</t>
   </si>
 </sst>
 </file>
@@ -234,12 +237,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -257,10 +263,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -571,7 +573,7 @@
     <col min="16" max="18" width="11.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,8 +643,11 @@
       <c r="W1" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="X1" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -715,8 +720,12 @@
         <f>I2/22</f>
         <v>75.694875038207272</v>
       </c>
+      <c r="X2">
+        <f>K2/4</f>
+        <v>50.58932959199975</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -789,8 +798,12 @@
         <f>I3/22</f>
         <v>74.106549498976818</v>
       </c>
+      <c r="X3">
+        <f>K3/4</f>
+        <v>50.696209771940147</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +861,7 @@
       </c>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -906,7 +919,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -964,15 +977,15 @@
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="L11" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="P15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="P16" t="s">
         <v>43</v>
       </c>

</xml_diff>